<commit_message>
Concentrado de metricas, reporte de monitoreo y minuta abril 15
</commit_message>
<xml_diff>
--- a/Organizacional/06. Medición y Monitoreo/2016/Acciones_Correctivas-2016.xlsx
+++ b/Organizacional/06. Medición y Monitoreo/2016/Acciones_Correctivas-2016.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Acciones Correctivas</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Jovanny Zepeda</t>
   </si>
   <si>
-    <t>Abierto</t>
+    <t>Cerrado</t>
   </si>
   <si>
     <t>Se presenta el riesgo de desviación en costos de proyectos.</t>
@@ -67,6 +67,9 @@
   <si>
     <t>Notificar a usuarios para la resolución de detalles y con evitar problemas futuros</t>
   </si>
+  <si>
+    <t>Dado que el proyecto ya ha alcanzado etapas altas se deberá estimar con mayor precisión, tomar como base lo aprendido de los primeros proyectos</t>
+  </si>
 </sst>
 </file>
 
@@ -74,10 +77,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$ &quot;* #,##0.00_-;&quot;-$ &quot;* #,##0.00_-;_-&quot;$ &quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -99,13 +102,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -149,6 +145,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -195,7 +192,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,15 +216,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,93 +226,73 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Moneda 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 2" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -393,15 +363,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>731880</xdr:colOff>
+      <xdr:colOff>785880</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>418320</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>824400</xdr:rowOff>
+      <xdr:rowOff>823680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -414,8 +384,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11705760" y="0"/>
-          <a:ext cx="3420360" cy="824400"/>
+          <a:off x="11759760" y="0"/>
+          <a:ext cx="3419640" cy="823680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -437,8 +407,8 @@
   </sheetPr>
   <dimension ref="1:28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3561,8 +3531,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="7"/>
+    <row r="5" customFormat="false" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
@@ -3578,13 +3550,17 @@
       <c r="H5" s="11" t="n">
         <v>42475</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="12" t="s">
+      <c r="I5" s="11" t="n">
+        <v>42475</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="10"/>
+    <row r="6" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
@@ -3600,13 +3576,17 @@
       <c r="H6" s="11" t="n">
         <v>42475</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="12" t="s">
+      <c r="I6" s="11" t="n">
+        <v>42475</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="10"/>
+    <row r="7" customFormat="false" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="12" t="n">
+        <v>3</v>
+      </c>
       <c r="D7" s="8" t="s">
         <v>15</v>
       </c>
@@ -3622,220 +3602,254 @@
       <c r="H7" s="11" t="n">
         <v>42475</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="12" t="s">
+      <c r="I7" s="11" t="n">
+        <v>42475</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="12"/>
+    <row r="8" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="13" t="n">
+        <v>42475</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="13" t="n">
+        <v>42475</v>
+      </c>
+      <c r="I8" s="13" t="n">
+        <v>42475</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="12"/>
+    <row r="9" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="13" t="n">
+        <v>42475</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="13" t="n">
+        <v>42475</v>
+      </c>
+      <c r="I9" s="13" t="n">
+        <v>42475</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="12"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="12"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="12"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="12"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="12"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
cambios plan de proyecto viaticos finales cambios acciones correctivas
</commit_message>
<xml_diff>
--- a/Organizacional/06. Medición y Monitoreo/2016/Acciones_Correctivas-2016.xlsx
+++ b/Organizacional/06. Medición y Monitoreo/2016/Acciones_Correctivas-2016.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Acciones Correctivas</t>
   </si>
@@ -69,6 +69,24 @@
   </si>
   <si>
     <t>Dado que el proyecto ya ha alcanzado etapas altas se deberá estimar con mayor precisión, tomar como base lo aprendido de los primeros proyectos</t>
+  </si>
+  <si>
+    <t>No se han realizado respaldos de la información</t>
+  </si>
+  <si>
+    <t>Realizar un respaldo inmediato, sin embargo se menciona que git hub tiene seguridad integrada y realiza respaldos de forma interna asegurando la estabilidad de información, esto se encuentra en sus políticas de seguridad</t>
+  </si>
+  <si>
+    <t>Abierto</t>
+  </si>
+  <si>
+    <t>No se ha realizado auditorías de monitoreo</t>
+  </si>
+  <si>
+    <t>Realizar la auditoría de monitoreo antes de la siguiente reunión de monitoreo</t>
+  </si>
+  <si>
+    <t>Vianey Castillo</t>
   </si>
 </sst>
 </file>
@@ -289,10 +307,22 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
     </dxf>
   </dxfs>
   <colors>
@@ -363,15 +393,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>785880</xdr:colOff>
+      <xdr:colOff>812880</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>471600</xdr:colOff>
+      <xdr:colOff>498240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823680</xdr:rowOff>
+      <xdr:rowOff>823320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -384,8 +414,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11759760" y="0"/>
-          <a:ext cx="3419640" cy="823680"/>
+          <a:off x="11786760" y="0"/>
+          <a:ext cx="3419280" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -408,7 +438,7 @@
   <dimension ref="1:28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3661,25 +3691,53 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+    <row r="10" customFormat="false" ht="58.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="13" t="n">
+        <v>42475</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="13" t="n">
+        <v>42490</v>
+      </c>
       <c r="I10" s="12"/>
-      <c r="J10" s="10"/>
+      <c r="J10" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+    <row r="11" customFormat="false" ht="30.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="13" t="n">
+        <v>42475</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="13" t="n">
+        <v>42490</v>
+      </c>
       <c r="I11" s="12"/>
-      <c r="J11" s="10"/>
+      <c r="J11" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="12"/>

</xml_diff>